<commit_message>
Update speeds.xlsx with new data
</commit_message>
<xml_diff>
--- a/speeds.xlsx
+++ b/speeds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellw\Desktop\Personal Projects\speedtestplot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134D3D3E-F134-4FFE-9BAE-0BA068C9BF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C49C39A-6B0C-4301-A644-882A9E778FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{EA806FDA-0D5E-4FE2-BB6C-58C6708B3DF4}"/>
+    <workbookView xWindow="3470" yWindow="2140" windowWidth="14400" windowHeight="7270" xr2:uid="{EA806FDA-0D5E-4FE2-BB6C-58C6708B3DF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,53 +36,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Device</t>
   </si>
   <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>Laptop - wifi</t>
-  </si>
-  <si>
-    <t>Laptop - RRC wifi</t>
-  </si>
-  <si>
-    <t>Laptop- Tethered</t>
-  </si>
-  <si>
-    <t>Laptop,Wi-Fi</t>
-  </si>
-  <si>
-    <t>LaptopRRC Wifi</t>
-  </si>
-  <si>
-    <t>Laptop RRC Wifi</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>laptop WIFI</t>
-  </si>
-  <si>
     <t>Laptop - Phone Tether</t>
   </si>
   <si>
-    <t xml:space="preserve">Laptop </t>
-  </si>
-  <si>
     <t>Shanghai</t>
   </si>
   <si>
     <t>Bell Canada</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>Ping</t>
   </si>
   <si>
@@ -119,9 +86,6 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>Pampa</t>
-  </si>
-  <si>
     <t>Tsukuba</t>
   </si>
   <si>
@@ -168,13 +132,22 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Laptop  - WIFI</t>
+  </si>
+  <si>
+    <t>Laptop - WIFI</t>
+  </si>
+  <si>
+    <t>Phone - Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,17 +164,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -235,7 +215,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A490126-079F-46F7-B343-7F2DBDB350E4}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,30 +585,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>42</v>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>228</v>
@@ -641,10 +622,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>329</v>
@@ -658,10 +639,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>16</v>
@@ -674,11 +655,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.4">
-      <c r="B5" s="5" t="s">
-        <v>32</v>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>328</v>
@@ -692,10 +673,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>220</v>
@@ -709,10 +690,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>397</v>
@@ -726,10 +707,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>395</v>
@@ -743,10 +724,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>24</v>
@@ -760,10 +741,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>214</v>
@@ -777,10 +758,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>347</v>
@@ -794,10 +775,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>161</v>
@@ -811,10 +792,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3">
         <v>565</v>
@@ -828,10 +809,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D14">
         <v>124</v>
@@ -845,10 +826,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>142</v>
@@ -862,10 +843,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>266</v>
@@ -879,10 +860,10 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D17">
         <v>247</v>
@@ -896,10 +877,10 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>164</v>
@@ -913,10 +894,10 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>295</v>
@@ -930,10 +911,10 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D20">
         <v>292</v>
@@ -947,10 +928,10 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D21">
         <v>310</v>
@@ -964,10 +945,10 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>310</v>
@@ -981,10 +962,10 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D23">
         <v>54</v>
@@ -998,10 +979,10 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D24">
         <v>167</v>
@@ -1015,10 +996,10 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D25">
         <v>224</v>
@@ -1032,10 +1013,10 @@
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>190</v>
@@ -1049,10 +1030,10 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D27">
         <v>38</v>
@@ -1066,10 +1047,10 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D28">
         <v>69</v>
@@ -1083,10 +1064,10 @@
     </row>
     <row r="29" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D29">
         <v>80</v>
@@ -1100,10 +1081,10 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D30">
         <v>123</v>
@@ -1116,11 +1097,11 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="4" t="s">
-        <v>27</v>
+      <c r="B31" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>99</v>

</xml_diff>